<commit_message>
edit hospital by Larisa
</commit_message>
<xml_diff>
--- a/docs/hospital.xlsx
+++ b/docs/hospital.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>hire_date</t>
   </si>
   <si>
-    <t>salary</t>
-  </si>
-  <si>
     <t>manager_id (FK)</t>
   </si>
   <si>
@@ -33,18 +30,6 @@
     <t>department_id (FK)</t>
   </si>
   <si>
-    <t>JOBS</t>
-  </si>
-  <si>
-    <t>job_id(PK)</t>
-  </si>
-  <si>
-    <t>job_title</t>
-  </si>
-  <si>
-    <t>job_category</t>
-  </si>
-  <si>
     <t>BLOOD_TYPE</t>
   </si>
   <si>
@@ -60,9 +45,6 @@
     <t>MEDICAL_RECORD</t>
   </si>
   <si>
-    <t>PATIENT</t>
-  </si>
-  <si>
     <t>EMPLOYEES</t>
   </si>
   <si>
@@ -123,9 +105,6 @@
     <t>personal_data_id (PK)</t>
   </si>
   <si>
-    <t>patient_id (PK)</t>
-  </si>
-  <si>
     <t>special_rates_id (PK)</t>
   </si>
   <si>
@@ -142,9 +121,6 @@
   </si>
   <si>
     <t>medical_record_id (FK)</t>
-  </si>
-  <si>
-    <t>patient_id (FK)</t>
   </si>
   <si>
     <t>personal_data_id (FK)</t>
@@ -359,50 +335,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="36" name="Прямая соединительная линия 35"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="952500" y="2314575"/>
-          <a:ext cx="0" cy="1295401"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>895349</xdr:colOff>
       <xdr:row>13</xdr:row>
@@ -453,7 +385,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>866775</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -463,7 +395,7 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="6619875" y="1352550"/>
-          <a:ext cx="19050" cy="923926"/>
+          <a:ext cx="19050" cy="742950"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -567,57 +499,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="49" name="Прямая соединительная линия 48"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5172075" y="2447925"/>
-          <a:ext cx="609600" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="4F81BD">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:srgbClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>19052</xdr:rowOff>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171452</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -626,8 +517,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="3676650" y="1905000"/>
-          <a:ext cx="9525" cy="590552"/>
+          <a:off x="3495675" y="1933575"/>
+          <a:ext cx="2447926" cy="333377"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -775,9 +666,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>971550</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
@@ -792,8 +683,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1581150" y="2352675"/>
-          <a:ext cx="2162176" cy="1666875"/>
+          <a:off x="1485900" y="2133600"/>
+          <a:ext cx="2257426" cy="1885950"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1617,129 +1508,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="37" name="Прямая соединительная линия 36"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1266825" y="3257550"/>
-          <a:ext cx="9525" cy="742950"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="4F81BD">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:srgbClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="38" name="Прямая соединительная линия 37"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1276350" y="3286125"/>
-          <a:ext cx="200025" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="4F81BD">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:srgbClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="39" name="Прямая соединительная линия 38"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1095375" y="3267075"/>
-          <a:ext cx="171450" cy="219075"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="4F81BD">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:srgbClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>895349</xdr:colOff>
       <xdr:row>20</xdr:row>
@@ -2232,231 +2000,108 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2124076</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1152526</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="77" name="Прямая соединительная линия 76"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5314950" y="1933575"/>
+          <a:ext cx="1143001" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="4F81BD">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:srgbClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1152525</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:colOff>904876</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="77" name="Прямая соединительная линия 76"/>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="Прямая соединительная линия 77"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6210301" y="2581275"/>
+          <a:ext cx="314324" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="4F81BD">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:srgbClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Прямая соединительная линия 78"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5295901" y="2705100"/>
-          <a:ext cx="1162049" cy="66675"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="4F81BD">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:srgbClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>981075</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1181100</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="78" name="Прямая соединительная линия 77"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="6286500" y="2733675"/>
-          <a:ext cx="200025" cy="142876"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="4F81BD">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:srgbClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1162050</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="79" name="Прямая соединительная линия 78"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="6219825" y="2590800"/>
-          <a:ext cx="247650" cy="133350"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="4F81BD">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:srgbClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="86" name="Прямая соединительная линия 85"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4124325" y="2124075"/>
-          <a:ext cx="0" cy="361951"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="4F81BD">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:srgbClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>971550</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1228725</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="87" name="Прямая соединительная линия 86"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4143375" y="2333625"/>
-          <a:ext cx="257175" cy="123825"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="4F81BD">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:srgbClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="88" name="Прямая соединительная линия 87"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3886200" y="2324100"/>
-          <a:ext cx="228600" cy="171450"/>
+          <a:off x="6210300" y="2543175"/>
+          <a:ext cx="314325" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3384,7 +3029,7 @@
   <dimension ref="B3:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3400,137 +3045,127 @@
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D7" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F9" s="2"/>
       <c r="H9" s="11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D11" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>1</v>
+      <c r="B12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
       <c r="F13" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G13" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="13">
-        <v>1</v>
-      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="12" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
       <c r="H15" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -3548,56 +3183,48 @@
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="12">
-        <v>1</v>
-      </c>
+      <c r="B19" s="12"/>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
-        <v>5</v>
-      </c>
+      <c r="B20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="B21" s="1"/>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="B22" s="1"/>
       <c r="D22" s="11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D23" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F24" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -3607,14 +3234,14 @@
       <c r="D26" s="1"/>
       <c r="F26" s="1"/>
       <c r="H26" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="H27" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
@@ -3632,7 +3259,7 @@
   <dimension ref="B1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3651,102 +3278,102 @@
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D6" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D7" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D9" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -3756,146 +3383,130 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D14" s="1"/>
       <c r="F14" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="1"/>
+      <c r="F15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="F16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="4" t="s">
+      <c r="H16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="D17" s="1"/>
       <c r="F17" s="8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F18" s="8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F19" s="8" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F20" s="9" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
       <c r="H21" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="D23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="D24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="D25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="D26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="F27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F28" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>